<commit_message>
changes to work around issue https://github.com/millennialmedia/intellibot/issues/111
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\markwinspear\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Google Drive\Documents\Dev &amp; Test\Robot Framework with Selenium\development\robot-scripts\data-driven-test\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14430" windowHeight="9630"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14436" windowHeight="9636"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -356,37 +356,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1">
+        <v>111</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
+      <c r="B2">
+        <v>222</v>
+      </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
+      <c r="B3">
+        <v>333</v>
+      </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
+      <c r="B4">
+        <v>444</v>
+      </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
+      </c>
+      <c r="B5">
+        <v>555</v>
       </c>
     </row>
   </sheetData>

</xml_diff>